<commit_message>
Minor changes to script and excel
</commit_message>
<xml_diff>
--- a/Result/hearing_age.xlsx
+++ b/Result/hearing_age.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Kvinder" sheetId="1" r:id="rId1"/>
@@ -41,21 +41,6 @@
     <t>Alder [år]</t>
   </si>
   <si>
-    <t>Ingen nedsættelse [≤]</t>
-  </si>
-  <si>
-    <t>Svag nedsættelse [≤]</t>
-  </si>
-  <si>
-    <t>Moderat nedsættelse [≤]</t>
-  </si>
-  <si>
-    <t>Alvorlig nedsættelse [≤]</t>
-  </si>
-  <si>
-    <t>Dybtgående nedsættelse [≥]</t>
-  </si>
-  <si>
     <t>10-19</t>
   </si>
   <si>
@@ -78,6 +63,21 @@
   </si>
   <si>
     <t>80-89</t>
+  </si>
+  <si>
+    <t>Moderat</t>
+  </si>
+  <si>
+    <t>Svag</t>
+  </si>
+  <si>
+    <t>Ingen</t>
+  </si>
+  <si>
+    <t>Alvorlig</t>
+  </si>
+  <si>
+    <t>Dybtgående</t>
   </si>
 </sst>
 </file>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -684,19 +684,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -704,7 +704,7 @@
         <v>0.25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7">
         <v>17.5</v>
@@ -731,7 +731,7 @@
         <v>0.25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7">
         <v>13.9</v>
@@ -758,7 +758,7 @@
         <v>0.25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="7">
         <v>15.8</v>
@@ -785,7 +785,7 @@
         <v>0.25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" s="7">
         <v>17.399999999999999</v>
@@ -812,7 +812,7 @@
         <v>0.25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" s="7">
         <v>19.5</v>
@@ -839,7 +839,7 @@
         <v>0.25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="7">
         <v>22.7</v>
@@ -866,7 +866,7 @@
         <v>0.25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="7">
         <v>29</v>
@@ -893,7 +893,7 @@
         <v>0.25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9" s="8">
         <v>30</v>
@@ -920,7 +920,7 @@
         <v>0.5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10" s="7">
         <v>15</v>
@@ -947,7 +947,7 @@
         <v>0.5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="7">
         <v>11.5</v>
@@ -974,7 +974,7 @@
         <v>0.5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C12" s="7">
         <v>12</v>
@@ -1001,7 +1001,7 @@
         <v>0.5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="7">
         <v>12.9</v>
@@ -1028,7 +1028,7 @@
         <v>0.5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C14" s="7">
         <v>16.100000000000001</v>
@@ -1055,7 +1055,7 @@
         <v>0.5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C15" s="7">
         <v>20.399999999999999</v>
@@ -1082,7 +1082,7 @@
         <v>0.5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16" s="7">
         <v>25.6</v>
@@ -1109,7 +1109,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C17" s="8">
         <v>33.799999999999997</v>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C18" s="7">
         <v>15</v>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C19" s="7">
         <v>8.5</v>
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20" s="7">
         <v>10.1</v>
@@ -1217,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21" s="7">
         <v>10.6</v>
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C22" s="7">
         <v>14.9</v>
@@ -1271,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C23" s="7">
         <v>21.4</v>
@@ -1298,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C24" s="7">
         <v>27.7</v>
@@ -1325,7 +1325,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C25" s="7">
         <v>32.5</v>
@@ -1352,7 +1352,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C26" s="6">
         <v>15</v>
@@ -1379,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C27" s="7">
         <v>5.6</v>
@@ -1406,7 +1406,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C28" s="7">
         <v>7.9</v>
@@ -1433,7 +1433,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C29" s="7">
         <v>9.4</v>
@@ -1460,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C30" s="7">
         <v>14.5</v>
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C31" s="7">
         <v>20.399999999999999</v>
@@ -1514,7 +1514,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C32" s="7">
         <v>31.7</v>
@@ -1541,7 +1541,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C33" s="8">
         <v>33.799999999999997</v>
@@ -1568,7 +1568,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C34" s="7">
         <v>15</v>
@@ -1595,7 +1595,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C35" s="7">
         <v>5.7</v>
@@ -1622,7 +1622,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C36" s="7">
         <v>9.6</v>
@@ -1649,7 +1649,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C37" s="7">
         <v>12.1</v>
@@ -1676,7 +1676,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C38" s="7">
         <v>19.2</v>
@@ -1703,7 +1703,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C39" s="7">
         <v>29.4</v>
@@ -1730,7 +1730,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C40" s="7">
         <v>41.7</v>
@@ -1757,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C41" s="8">
         <v>38.799999999999997</v>
@@ -1784,7 +1784,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C42" s="7">
         <v>13.8</v>
@@ -1811,7 +1811,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C43" s="7">
         <v>6.9</v>
@@ -1838,7 +1838,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44" s="7">
         <v>13.1</v>
@@ -1865,7 +1865,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45" s="7">
         <v>16.899999999999999</v>
@@ -1892,7 +1892,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" s="7">
         <v>29.4</v>
@@ -1919,7 +1919,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C47" s="7">
         <v>45.7</v>
@@ -1946,7 +1946,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C48" s="7">
         <v>63.7</v>
@@ -1973,7 +1973,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C49" s="8">
         <v>56.3</v>
@@ -2004,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2026,19 +2026,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2046,7 +2046,7 @@
         <v>0.25</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" s="14">
         <v>10.8</v>
@@ -2073,7 +2073,7 @@
         <v>0.25</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="15">
         <v>11</v>
@@ -2100,7 +2100,7 @@
         <v>0.25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" s="15">
         <v>16.3</v>
@@ -2127,7 +2127,7 @@
         <v>0.25</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" s="15">
         <v>17.5</v>
@@ -2154,7 +2154,7 @@
         <v>0.25</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" s="15">
         <v>18.899999999999999</v>
@@ -2181,7 +2181,7 @@
         <v>0.25</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="15">
         <v>23.8</v>
@@ -2208,7 +2208,7 @@
         <v>0.25</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="15">
         <v>25</v>
@@ -2235,7 +2235,7 @@
         <v>0.25</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="12"/>
@@ -2248,7 +2248,7 @@
         <v>0.5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C10" s="15">
         <v>12.6</v>
@@ -2275,7 +2275,7 @@
         <v>0.5</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="15">
         <v>7.5</v>
@@ -2302,7 +2302,7 @@
         <v>0.5</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C12" s="15">
         <v>12.3</v>
@@ -2329,7 +2329,7 @@
         <v>0.5</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C13" s="15">
         <v>14.1</v>
@@ -2356,7 +2356,7 @@
         <v>0.5</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C14" s="15">
         <v>15</v>
@@ -2383,7 +2383,7 @@
         <v>0.5</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C15" s="15">
         <v>19.100000000000001</v>
@@ -2410,7 +2410,7 @@
         <v>0.5</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16" s="15">
         <v>25.6</v>
@@ -2437,7 +2437,7 @@
         <v>0.5</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C17" s="15">
         <v>6.7</v>
@@ -2464,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C18" s="14">
         <v>5.5</v>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C19" s="15">
         <v>10.199999999999999</v>
@@ -2518,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20" s="15">
         <v>12.9</v>
@@ -2545,7 +2545,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21" s="15">
         <v>15.3</v>
@@ -2572,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C22" s="15">
         <v>18.8</v>
@@ -2599,7 +2599,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C23" s="15">
         <v>26.3</v>
@@ -2626,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="11"/>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="12"/>
@@ -2652,7 +2652,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C26" s="15">
         <v>2.5</v>
@@ -2679,7 +2679,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C27" s="15">
         <v>2.5</v>
@@ -2706,7 +2706,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C28" s="15">
         <v>6.4</v>
@@ -2733,7 +2733,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C29" s="15">
         <v>11.1</v>
@@ -2760,7 +2760,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C30" s="15">
         <v>14.3</v>
@@ -2787,7 +2787,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C31" s="15">
         <v>22.7</v>
@@ -2814,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C32" s="15">
         <v>24.2</v>
@@ -2841,7 +2841,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="11"/>
@@ -2854,7 +2854,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C34" s="14">
         <v>3.3</v>
@@ -2881,7 +2881,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="11"/>
@@ -2894,7 +2894,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C36" s="15">
         <v>11.9</v>
@@ -2921,7 +2921,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C37" s="15">
         <v>22.2</v>
@@ -2948,7 +2948,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C38" s="15">
         <v>25.7</v>
@@ -2975,7 +2975,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C39" s="15">
         <v>41</v>
@@ -3002,7 +3002,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C40" s="15">
         <v>38.799999999999997</v>
@@ -3029,7 +3029,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C41" s="16">
         <v>3.3</v>
@@ -3056,7 +3056,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C42" s="15">
         <v>5.5</v>
@@ -3083,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C43" s="15">
         <v>14.8</v>
@@ -3110,7 +3110,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44" s="15">
         <v>25.4</v>
@@ -3137,7 +3137,7 @@
         <v>8</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45" s="15">
         <v>31.7</v>
@@ -3164,7 +3164,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" s="15">
         <v>57.9</v>
@@ -3191,7 +3191,7 @@
         <v>8</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C47" s="15">
         <v>58.8</v>
@@ -3218,7 +3218,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="11"/>
@@ -3231,7 +3231,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="12"/>

</xml_diff>

<commit_message>
Changed result.py and modified excel sheet
</commit_message>
<xml_diff>
--- a/Result/hearing_age.xlsx
+++ b/Result/hearing_age.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kvinder" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="16">
   <si>
     <t>Frekvens [kHz]</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Dybtgående</t>
+  </si>
+  <si>
+    <t>Frekvens [Hz]</t>
   </si>
 </sst>
 </file>
@@ -209,19 +212,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -266,15 +256,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
@@ -301,53 +308,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -678,30 +674,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="20">
-        <v>0.25</v>
+      <c r="A2" s="25">
+        <v>250</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
@@ -727,8 +723,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
-        <v>0.25</v>
+      <c r="A3" s="26">
+        <v>250</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -754,8 +750,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="17">
-        <v>0.25</v>
+      <c r="A4" s="26">
+        <v>250</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -781,8 +777,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
-        <v>0.25</v>
+      <c r="A5" s="26">
+        <v>250</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -808,8 +804,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
-        <v>0.25</v>
+      <c r="A6" s="26">
+        <v>250</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -835,8 +831,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
-        <v>0.25</v>
+      <c r="A7" s="26">
+        <v>250</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -862,8 +858,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="17">
-        <v>0.25</v>
+      <c r="A8" s="26">
+        <v>250</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -890,7 +886,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
-        <v>0.25</v>
+        <v>250</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -917,7 +913,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
@@ -944,7 +940,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -971,7 +967,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -998,7 +994,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1025,7 +1021,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
@@ -1052,7 +1048,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
@@ -1079,7 +1075,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -1106,7 +1102,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
-        <v>0.5</v>
+        <v>500</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
@@ -1132,8 +1128,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="21">
-        <v>1</v>
+      <c r="A18" s="25">
+        <v>1000</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>2</v>
@@ -1159,8 +1155,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
-        <v>1</v>
+      <c r="A19" s="26">
+        <v>1000</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -1186,8 +1182,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="17">
-        <v>1</v>
+      <c r="A20" s="26">
+        <v>1000</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
@@ -1213,8 +1209,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="17">
-        <v>1</v>
+      <c r="A21" s="26">
+        <v>1000</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
@@ -1240,8 +1236,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="17">
-        <v>1</v>
+      <c r="A22" s="26">
+        <v>1000</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -1267,8 +1263,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="17">
-        <v>1</v>
+      <c r="A23" s="26">
+        <v>1000</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
@@ -1294,8 +1290,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="17">
-        <v>1</v>
+      <c r="A24" s="27">
+        <v>1000</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1321,8 +1317,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="17">
-        <v>1</v>
+      <c r="A25" s="28">
+        <v>1000</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -1348,8 +1344,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="20">
-        <v>2</v>
+      <c r="A26" s="26">
+        <v>2000</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>2</v>
@@ -1375,8 +1371,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="17">
-        <v>2</v>
+      <c r="A27" s="26">
+        <v>2000</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -1402,8 +1398,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="17">
-        <v>2</v>
+      <c r="A28" s="26">
+        <v>2000</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
@@ -1429,8 +1425,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="17">
-        <v>2</v>
+      <c r="A29" s="26">
+        <v>2000</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
@@ -1456,8 +1452,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="17">
-        <v>2</v>
+      <c r="A30" s="26">
+        <v>2000</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -1483,8 +1479,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="17">
-        <v>2</v>
+      <c r="A31" s="26">
+        <v>2000</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
@@ -1510,8 +1506,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="17">
-        <v>2</v>
+      <c r="A32" s="26">
+        <v>2000</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
@@ -1537,8 +1533,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="18">
-        <v>2</v>
+      <c r="A33" s="29">
+        <v>2000</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>9</v>
@@ -1565,7 +1561,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>2</v>
@@ -1592,7 +1588,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
@@ -1619,7 +1615,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
@@ -1646,7 +1642,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>5</v>
@@ -1673,7 +1669,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>6</v>
@@ -1700,7 +1696,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -1727,7 +1723,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="17">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>8</v>
@@ -1753,8 +1749,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="18">
-        <v>4</v>
+      <c r="A41" s="24">
+        <v>4000</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>9</v>
@@ -1781,7 +1777,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>2</v>
@@ -1808,7 +1804,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>3</v>
@@ -1835,7 +1831,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>4</v>
@@ -1862,7 +1858,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>5</v>
@@ -1889,7 +1885,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>6</v>
@@ -1916,7 +1912,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
@@ -1943,7 +1939,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="17">
-        <v>8</v>
+        <v>8000</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>8</v>
@@ -1969,8 +1965,8 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="18">
-        <v>8</v>
+      <c r="A49" s="24">
+        <v>8000</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>9</v>
@@ -2004,8 +2000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2019,13 +2015,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="22" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="11" t="s">
@@ -2042,8 +2038,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="24">
-        <v>0.25</v>
+      <c r="A2" s="25">
+        <v>250</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>2</v>
@@ -2069,8 +2065,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="25">
-        <v>0.25</v>
+      <c r="A3" s="26">
+        <v>250</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>3</v>
@@ -2096,8 +2092,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="25">
-        <v>0.25</v>
+      <c r="A4" s="26">
+        <v>250</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>4</v>
@@ -2123,8 +2119,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="25">
-        <v>0.25</v>
+      <c r="A5" s="26">
+        <v>250</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>5</v>
@@ -2150,8 +2146,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
-        <v>0.25</v>
+      <c r="A6" s="26">
+        <v>250</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>6</v>
@@ -2177,8 +2173,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="25">
-        <v>0.25</v>
+      <c r="A7" s="26">
+        <v>250</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>7</v>
@@ -2204,8 +2200,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="25">
-        <v>0.25</v>
+      <c r="A8" s="26">
+        <v>250</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>8</v>
@@ -2231,8 +2227,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="25">
-        <v>0.25</v>
+      <c r="A9" s="18">
+        <v>250</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>9</v>
@@ -2244,8 +2240,8 @@
       <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="31">
-        <v>0.5</v>
+      <c r="A10" s="17">
+        <v>500</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>2</v>
@@ -2271,8 +2267,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="32">
-        <v>0.5</v>
+      <c r="A11" s="17">
+        <v>500</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>3</v>
@@ -2298,8 +2294,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="32">
-        <v>0.5</v>
+      <c r="A12" s="17">
+        <v>500</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>4</v>
@@ -2325,8 +2321,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="32">
-        <v>0.5</v>
+      <c r="A13" s="17">
+        <v>500</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>5</v>
@@ -2352,8 +2348,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="32">
-        <v>0.5</v>
+      <c r="A14" s="17">
+        <v>500</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>6</v>
@@ -2379,8 +2375,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="33">
-        <v>0.5</v>
+      <c r="A15" s="17">
+        <v>500</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>7</v>
@@ -2406,8 +2402,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="33">
-        <v>0.5</v>
+      <c r="A16" s="17">
+        <v>500</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>8</v>
@@ -2433,8 +2429,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="34">
-        <v>0.5</v>
+      <c r="A17" s="17">
+        <v>500</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>9</v>
@@ -2460,8 +2456,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="27">
-        <v>1</v>
+      <c r="A18" s="25">
+        <v>1000</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>2</v>
@@ -2487,8 +2483,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="27">
-        <v>1</v>
+      <c r="A19" s="26">
+        <v>1000</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>3</v>
@@ -2514,8 +2510,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="27">
-        <v>1</v>
+      <c r="A20" s="26">
+        <v>1000</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>4</v>
@@ -2541,8 +2537,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="27">
-        <v>1</v>
+      <c r="A21" s="26">
+        <v>1000</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>5</v>
@@ -2568,8 +2564,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="27">
-        <v>1</v>
+      <c r="A22" s="26">
+        <v>1000</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>6</v>
@@ -2595,8 +2591,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="27">
-        <v>1</v>
+      <c r="A23" s="26">
+        <v>1000</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>7</v>
@@ -2623,7 +2619,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>8</v>
@@ -2636,7 +2632,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="28">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>9</v>
@@ -2649,7 +2645,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="26">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>2</v>
@@ -2675,8 +2671,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="27">
-        <v>2</v>
+      <c r="A27" s="26">
+        <v>2000</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>3</v>
@@ -2702,8 +2698,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="27">
-        <v>2</v>
+      <c r="A28" s="26">
+        <v>2000</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>4</v>
@@ -2729,8 +2725,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="27">
-        <v>2</v>
+      <c r="A29" s="26">
+        <v>2000</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>5</v>
@@ -2756,8 +2752,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="27">
-        <v>2</v>
+      <c r="A30" s="26">
+        <v>2000</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>6</v>
@@ -2783,8 +2779,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="27">
-        <v>2</v>
+      <c r="A31" s="26">
+        <v>2000</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>7</v>
@@ -2810,8 +2806,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="27">
-        <v>2</v>
+      <c r="A32" s="26">
+        <v>2000</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>8</v>
@@ -2837,8 +2833,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="28">
-        <v>2</v>
+      <c r="A33" s="29">
+        <v>2000</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>9</v>
@@ -2850,8 +2846,8 @@
       <c r="G33" s="15"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="26">
-        <v>4</v>
+      <c r="A34" s="17">
+        <v>4000</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>2</v>
@@ -2877,8 +2873,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="27">
-        <v>4</v>
+      <c r="A35" s="17">
+        <v>4000</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>3</v>
@@ -2890,8 +2886,8 @@
       <c r="G35" s="15"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="27">
-        <v>4</v>
+      <c r="A36" s="17">
+        <v>4000</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>4</v>
@@ -2917,8 +2913,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="27">
-        <v>4</v>
+      <c r="A37" s="17">
+        <v>4000</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>5</v>
@@ -2944,8 +2940,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="27">
-        <v>4</v>
+      <c r="A38" s="17">
+        <v>4000</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>6</v>
@@ -2971,8 +2967,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="27">
-        <v>4</v>
+      <c r="A39" s="17">
+        <v>4000</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>7</v>
@@ -2998,8 +2994,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="27">
-        <v>4</v>
+      <c r="A40" s="17">
+        <v>4000</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>8</v>
@@ -3025,8 +3021,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="28">
-        <v>4</v>
+      <c r="A41" s="24">
+        <v>4000</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>9</v>
@@ -3052,8 +3048,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="26">
-        <v>8</v>
+      <c r="A42" s="17">
+        <v>8000</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>2</v>
@@ -3079,8 +3075,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="27">
-        <v>8</v>
+      <c r="A43" s="17">
+        <v>8000</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>3</v>
@@ -3106,8 +3102,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="27">
-        <v>8</v>
+      <c r="A44" s="17">
+        <v>8000</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>4</v>
@@ -3133,8 +3129,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="27">
-        <v>8</v>
+      <c r="A45" s="17">
+        <v>8000</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>5</v>
@@ -3160,8 +3156,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="27">
-        <v>8</v>
+      <c r="A46" s="17">
+        <v>8000</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>6</v>
@@ -3187,8 +3183,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="27">
-        <v>8</v>
+      <c r="A47" s="17">
+        <v>8000</v>
       </c>
       <c r="B47" s="11" t="s">
         <v>7</v>
@@ -3214,8 +3210,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="27">
-        <v>8</v>
+      <c r="A48" s="17">
+        <v>8000</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>8</v>
@@ -3227,8 +3223,8 @@
       <c r="G48" s="15"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="28">
-        <v>8</v>
+      <c r="A49" s="24">
+        <v>8000</v>
       </c>
       <c r="B49" s="12" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Update to calculate result, and GUI
</commit_message>
<xml_diff>
--- a/Result/hearing_age.xlsx
+++ b/Result/hearing_age.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnusborresen/Documents/AAU_EIT/1-Semester/P1/p1_project/Result/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krist\p1_project\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E626E9A1-CC14-481F-8E45-C182E8839B6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kvinder" sheetId="1" r:id="rId1"/>
     <sheet name="Maend" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -23,20 +24,12 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="16">
-  <si>
-    <t>Frekvens [kHz]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="15">
   <si>
     <t>Alder [år]</t>
   </si>
@@ -86,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,10 +333,10 @@
     <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -655,52 +648,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A49"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="25">
         <v>250</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="7">
         <v>17.5</v>
@@ -722,12 +715,12 @@
         <v>56.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>250</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="7">
         <v>13.9</v>
@@ -749,12 +742,12 @@
         <v>45.036000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="26">
         <v>250</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="7">
         <v>15.8</v>
@@ -776,12 +769,12 @@
         <v>51.192000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>250</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="7">
         <v>17.399999999999999</v>
@@ -803,12 +796,12 @@
         <v>56.375999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>250</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7">
         <v>19.5</v>
@@ -830,12 +823,12 @@
         <v>63.180000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>250</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7">
         <v>22.7</v>
@@ -857,12 +850,12 @@
         <v>73.548000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>250</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="7">
         <v>29</v>
@@ -884,12 +877,12 @@
         <v>93.960000000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>250</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8">
         <v>30</v>
@@ -911,12 +904,12 @@
         <v>97.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="17">
         <v>500</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="7">
         <v>15</v>
@@ -938,12 +931,12 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>500</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="7">
         <v>11.5</v>
@@ -965,12 +958,12 @@
         <v>37.260000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17">
         <v>500</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="7">
         <v>12</v>
@@ -992,12 +985,12 @@
         <v>38.880000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="17">
         <v>500</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="7">
         <v>12.9</v>
@@ -1019,12 +1012,12 @@
         <v>41.796000000000006</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="17">
         <v>500</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="7">
         <v>16.100000000000001</v>
@@ -1046,12 +1039,12 @@
         <v>52.164000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="17">
         <v>500</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="7">
         <v>20.399999999999999</v>
@@ -1073,12 +1066,12 @@
         <v>66.096000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="17">
         <v>500</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="7">
         <v>25.6</v>
@@ -1100,12 +1093,12 @@
         <v>82.944000000000017</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="17">
         <v>500</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8">
         <v>33.799999999999997</v>
@@ -1127,12 +1120,12 @@
         <v>109.512</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
         <v>1000</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="7">
         <v>15</v>
@@ -1154,12 +1147,12 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="26">
         <v>1000</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="7">
         <v>8.5</v>
@@ -1181,12 +1174,12 @@
         <v>27.540000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="26">
         <v>1000</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="7">
         <v>10.1</v>
@@ -1208,12 +1201,12 @@
         <v>32.724000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="26">
         <v>1000</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="7">
         <v>10.6</v>
@@ -1235,12 +1228,12 @@
         <v>34.344000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="26">
         <v>1000</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="7">
         <v>14.9</v>
@@ -1262,12 +1255,12 @@
         <v>48.276000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="26">
         <v>1000</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="7">
         <v>21.4</v>
@@ -1289,12 +1282,12 @@
         <v>69.335999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="27">
         <v>1000</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="7">
         <v>27.7</v>
@@ -1316,12 +1309,12 @@
         <v>89.748000000000005</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="28">
         <v>1000</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="7">
         <v>32.5</v>
@@ -1343,12 +1336,12 @@
         <v>105.30000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="26">
         <v>2000</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="6">
         <v>15</v>
@@ -1370,12 +1363,12 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="26">
         <v>2000</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="7">
         <v>5.6</v>
@@ -1397,12 +1390,12 @@
         <v>18.143999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>2000</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="7">
         <v>7.9</v>
@@ -1424,12 +1417,12 @@
         <v>25.596000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="26">
         <v>2000</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="7">
         <v>9.4</v>
@@ -1451,12 +1444,12 @@
         <v>30.456000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="26">
         <v>2000</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="7">
         <v>14.5</v>
@@ -1478,12 +1471,12 @@
         <v>46.980000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="26">
         <v>2000</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="7">
         <v>20.399999999999999</v>
@@ -1505,12 +1498,12 @@
         <v>66.096000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>2000</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="7">
         <v>31.7</v>
@@ -1532,12 +1525,12 @@
         <v>102.708</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="29">
         <v>2000</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="8">
         <v>33.799999999999997</v>
@@ -1559,12 +1552,12 @@
         <v>109.512</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="17">
         <v>4000</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="7">
         <v>15</v>
@@ -1586,12 +1579,12 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="17">
         <v>4000</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="7">
         <v>5.7</v>
@@ -1613,12 +1606,12 @@
         <v>18.468000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="17">
         <v>4000</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="7">
         <v>9.6</v>
@@ -1640,12 +1633,12 @@
         <v>31.103999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="17">
         <v>4000</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="7">
         <v>12.1</v>
@@ -1667,12 +1660,12 @@
         <v>39.204000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="17">
         <v>4000</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="7">
         <v>19.2</v>
@@ -1694,12 +1687,12 @@
         <v>62.207999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="17">
         <v>4000</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="7">
         <v>29.4</v>
@@ -1721,12 +1714,12 @@
         <v>95.256</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="17">
         <v>4000</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="7">
         <v>41.7</v>
@@ -1748,12 +1741,12 @@
         <v>135.108</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="24">
         <v>4000</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="8">
         <v>38.799999999999997</v>
@@ -1775,12 +1768,12 @@
         <v>125.712</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="17">
         <v>8000</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="7">
         <v>13.8</v>
@@ -1802,12 +1795,12 @@
         <v>44.712000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="17">
         <v>8000</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="7">
         <v>6.9</v>
@@ -1829,12 +1822,12 @@
         <v>22.356000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="17">
         <v>8000</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="7">
         <v>13.1</v>
@@ -1856,12 +1849,12 @@
         <v>42.444000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="17">
         <v>8000</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="7">
         <v>16.899999999999999</v>
@@ -1883,12 +1876,12 @@
         <v>54.756</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="17">
         <v>8000</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="7">
         <v>29.4</v>
@@ -1910,12 +1903,12 @@
         <v>95.256</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="17">
         <v>8000</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" s="7">
         <v>45.7</v>
@@ -1937,12 +1930,12 @@
         <v>148.06800000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="17">
         <v>8000</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="7">
         <v>63.7</v>
@@ -1964,12 +1957,12 @@
         <v>206.38800000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="24">
         <v>8000</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="8">
         <v>56.3</v>
@@ -1997,52 +1990,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="25">
         <v>250</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="14">
         <v>10.8</v>
@@ -2064,12 +2057,12 @@
         <v>34.992000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="26">
         <v>250</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="15">
         <v>11</v>
@@ -2091,12 +2084,12 @@
         <v>35.64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="26">
         <v>250</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="15">
         <v>16.3</v>
@@ -2118,12 +2111,12 @@
         <v>52.812000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="26">
         <v>250</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="15">
         <v>17.5</v>
@@ -2145,12 +2138,12 @@
         <v>56.7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="26">
         <v>250</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="15">
         <v>18.899999999999999</v>
@@ -2172,12 +2165,12 @@
         <v>61.235999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>250</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="15">
         <v>23.8</v>
@@ -2199,12 +2192,12 @@
         <v>77.112000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="26">
         <v>250</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="15">
         <v>25</v>
@@ -2226,12 +2219,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>250</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="12"/>
@@ -2239,12 +2232,12 @@
       <c r="F9" s="12"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="17">
         <v>500</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="15">
         <v>12.6</v>
@@ -2266,12 +2259,12 @@
         <v>40.823999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>500</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="15">
         <v>7.5</v>
@@ -2293,12 +2286,12 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="17">
         <v>500</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" s="15">
         <v>12.3</v>
@@ -2320,12 +2313,12 @@
         <v>39.852000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="17">
         <v>500</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="15">
         <v>14.1</v>
@@ -2347,12 +2340,12 @@
         <v>45.684000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="17">
         <v>500</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="15">
         <v>15</v>
@@ -2374,12 +2367,12 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="17">
         <v>500</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="15">
         <v>19.100000000000001</v>
@@ -2401,12 +2394,12 @@
         <v>61.884000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="17">
         <v>500</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="15">
         <v>25.6</v>
@@ -2428,12 +2421,12 @@
         <v>82.944000000000017</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="17">
         <v>500</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="15">
         <v>6.7</v>
@@ -2455,12 +2448,12 @@
         <v>21.708000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="25">
         <v>1000</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="14">
         <v>5.5</v>
@@ -2482,12 +2475,12 @@
         <v>17.82</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="26">
         <v>1000</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="15">
         <v>10.199999999999999</v>
@@ -2509,12 +2502,12 @@
         <v>33.048000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="26">
         <v>1000</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="15">
         <v>12.9</v>
@@ -2536,12 +2529,12 @@
         <v>41.796000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="26">
         <v>1000</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="15">
         <v>15.3</v>
@@ -2563,12 +2556,12 @@
         <v>49.572000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="26">
         <v>1000</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="15">
         <v>18.8</v>
@@ -2590,12 +2583,12 @@
         <v>60.912000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="26">
         <v>1000</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="15">
         <v>26.3</v>
@@ -2617,12 +2610,12 @@
         <v>85.212000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="27">
         <v>1000</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="11"/>
@@ -2630,12 +2623,12 @@
       <c r="F24" s="11"/>
       <c r="G24" s="15"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="28">
         <v>1000</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="16"/>
       <c r="D25" s="12"/>
@@ -2643,12 +2636,12 @@
       <c r="F25" s="12"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="26">
         <v>2000</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="15">
         <v>2.5</v>
@@ -2670,12 +2663,12 @@
         <v>8.1000000000000014</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="26">
         <v>2000</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="15">
         <v>2.5</v>
@@ -2697,12 +2690,12 @@
         <v>8.1000000000000014</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="26">
         <v>2000</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="15">
         <v>6.4</v>
@@ -2724,12 +2717,12 @@
         <v>20.736000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="26">
         <v>2000</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="15">
         <v>11.1</v>
@@ -2751,12 +2744,12 @@
         <v>35.963999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="26">
         <v>2000</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="15">
         <v>14.3</v>
@@ -2778,12 +2771,12 @@
         <v>46.332000000000008</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="26">
         <v>2000</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="15">
         <v>22.7</v>
@@ -2805,12 +2798,12 @@
         <v>73.548000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>2000</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="15">
         <v>24.2</v>
@@ -2832,12 +2825,12 @@
         <v>78.408000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="29">
         <v>2000</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="11"/>
@@ -2845,12 +2838,12 @@
       <c r="F33" s="11"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="17">
         <v>4000</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="14">
         <v>3.3</v>
@@ -2872,12 +2865,12 @@
         <v>10.692</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="17">
         <v>4000</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="11"/>
@@ -2885,12 +2878,12 @@
       <c r="F35" s="11"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="17">
         <v>4000</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" s="15">
         <v>11.9</v>
@@ -2912,12 +2905,12 @@
         <v>38.556000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="17">
         <v>4000</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="15">
         <v>22.2</v>
@@ -2939,12 +2932,12 @@
         <v>71.927999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="17">
         <v>4000</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="15">
         <v>25.7</v>
@@ -2966,12 +2959,12 @@
         <v>83.268000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="17">
         <v>4000</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="15">
         <v>41</v>
@@ -2993,12 +2986,12 @@
         <v>132.84</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="17">
         <v>4000</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="15">
         <v>38.799999999999997</v>
@@ -3020,12 +3013,12 @@
         <v>125.712</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="24">
         <v>4000</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C41" s="16">
         <v>3.3</v>
@@ -3047,12 +3040,12 @@
         <v>10.692</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="17">
         <v>8000</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="15">
         <v>5.5</v>
@@ -3074,12 +3067,12 @@
         <v>17.82</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="17">
         <v>8000</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="15">
         <v>14.8</v>
@@ -3101,12 +3094,12 @@
         <v>47.952000000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="17">
         <v>8000</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C44" s="15">
         <v>25.4</v>
@@ -3128,12 +3121,12 @@
         <v>82.296000000000006</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="17">
         <v>8000</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" s="15">
         <v>31.7</v>
@@ -3155,12 +3148,12 @@
         <v>102.708</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="17">
         <v>8000</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="15">
         <v>57.9</v>
@@ -3182,12 +3175,12 @@
         <v>187.596</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="17">
         <v>8000</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" s="15">
         <v>58.8</v>
@@ -3209,12 +3202,12 @@
         <v>190.512</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="17">
         <v>8000</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="11"/>
@@ -3222,12 +3215,12 @@
       <c r="F48" s="11"/>
       <c r="G48" s="15"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="24">
         <v>8000</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" s="16"/>
       <c r="D49" s="12"/>

</xml_diff>